<commit_message>
New datas: 	generate2, 86%, less complex, 4 veces more low 	generate, 62%, more complex, 4 veces more fast
</commit_message>
<xml_diff>
--- a/resources/pseudoalgoritmo para crear sudokus.xlsx
+++ b/resources/pseudoalgoritmo para crear sudokus.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="pseudoalgoritmo" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="test" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -535,15 +536,15 @@
   </sheetPr>
   <dimension ref="A1:T243"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N16" activeCellId="0" sqref="N16"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="5.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1694,10 +1695,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="3.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="4.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="29" style="0" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="4.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="29" style="0" width="3.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1733,7 +1734,7 @@
       </c>
       <c r="AB1" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,9)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1795,7 +1796,7 @@
       </c>
       <c r="AB2" s="0" t="n">
         <f aca="false">RANDBETWEEN(0,8)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2588,4 +2589,30 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>